<commit_message>
updated US map & data
</commit_message>
<xml_diff>
--- a/data/excel/BLS_Total_Women_Men_2020.xlsx
+++ b/data/excel/BLS_Total_Women_Men_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\TAMU\Fall '21\Data Visualization\Project\Repo\wage-gap\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Texas A&amp;M\Senior\Fall 2021\CSCE 447 - Data Visualization\wage-gap\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292C5BFB-E711-48A1-8903-0ABF898D72D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23174605-687E-4717-9EC1-75BDA91FF8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C29C535-010B-AB46-B1F7-F30D4DD0FF61}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{5C29C535-010B-AB46-B1F7-F30D4DD0FF61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464A82E6-7F63-514E-8938-2ECCCC748C0D}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -737,16 +737,16 @@
         <v>80.900000000000006</v>
       </c>
       <c r="M2" s="4">
-        <f t="shared" ref="M2:M52" si="0">(J2-G2)/((G2+J2)/2)</f>
-        <v>0.21141888072357265</v>
+        <f>(J2-G2)/((G2+J2)/2)*100</f>
+        <v>21.141888072357265</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N52" si="1">(I2-F2)/(C2/2)</f>
-        <v>0.17076167076167076</v>
+        <f>(I2-F2)/(C2/2)*100</f>
+        <v>17.076167076167074</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O52" si="2">(K2-H2)/((K2+H2)/2)</f>
-        <v>0.32</v>
+        <f>(K2-H2)/((K2+H2)/2)*100</f>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -787,15 +787,15 @@
         <v>80.900000000000006</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" si="0"/>
-        <v>0.21068103870651642</v>
+        <f t="shared" ref="M3:M52" si="0">(J3-G3)/((G3+J3)/2)*100</f>
+        <v>21.06810387065164</v>
       </c>
       <c r="N3">
-        <f t="shared" si="1"/>
-        <v>0.21848739495798319</v>
+        <f t="shared" ref="N3:N52" si="1">(I3-F3)/(C3/2)*100</f>
+        <v>21.84873949579832</v>
       </c>
       <c r="O3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="O3:O52" si="2">(K3-H3)/((K3+H3)/2)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -838,15 +838,15 @@
       </c>
       <c r="M4" s="4">
         <f t="shared" si="0"/>
-        <v>0.14618299945858149</v>
+        <v>14.618299945858148</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>0.20050335570469799</v>
+        <v>20.050335570469798</v>
       </c>
       <c r="O4">
         <f t="shared" si="2"/>
-        <v>-0.60465116279069764</v>
+        <v>-60.465116279069761</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -888,15 +888,15 @@
       </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>0.17298578199052134</v>
+        <v>17.298578199052134</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>0.21909547738693466</v>
+        <v>21.909547738693465</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>0.21052631578947367</v>
+        <v>21.052631578947366</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -938,15 +938,15 @@
       </c>
       <c r="M6" s="4">
         <f t="shared" si="0"/>
-        <v>0.13170272812793979</v>
+        <v>13.170272812793979</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>0.27774234693877553</v>
+        <v>27.774234693877553</v>
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>15.384615384615385</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -988,15 +988,15 @@
       </c>
       <c r="M7" s="4">
         <f t="shared" si="0"/>
-        <v>0.2460281434407626</v>
+        <v>24.602814344076261</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>0.3386454183266932</v>
+        <v>33.864541832669318</v>
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>-0.34146341463414637</v>
+        <v>-34.146341463414636</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1038,15 +1038,15 @@
       </c>
       <c r="M8" s="4">
         <f t="shared" si="0"/>
-        <v>3.0405405405405407E-2</v>
+        <v>3.0405405405405408</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0.24242424242424243</v>
+        <v>24.242424242424242</v>
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>-0.38709677419354838</v>
+        <v>-38.70967741935484</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1088,15 +1088,15 @@
       </c>
       <c r="M9" s="4">
         <f t="shared" si="0"/>
-        <v>0.24869383490073146</v>
+        <v>24.869383490073147</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>0.12290502793296089</v>
+        <v>12.290502793296088</v>
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>0.76595744680851063</v>
+        <v>76.59574468085107</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1138,15 +1138,15 @@
       </c>
       <c r="M10" s="4">
         <f t="shared" si="0"/>
-        <v>0.15497702909647779</v>
+        <v>15.497702909647778</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>-6.4308681672025723E-3</v>
+        <v>-0.64308681672025725</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>-0.29213483146067415</v>
+        <v>-29.213483146067414</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1188,15 +1188,15 @@
       </c>
       <c r="M11" s="4">
         <f t="shared" si="0"/>
-        <v>0.17262231995601979</v>
+        <v>17.262231995601979</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>0.1500355871886121</v>
+        <v>15.003558718861211</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>0.18181818181818182</v>
+        <v>18.181818181818183</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1238,15 +1238,15 @@
       </c>
       <c r="M12" s="4">
         <f t="shared" si="0"/>
-        <v>0.24791550861589773</v>
+        <v>24.791550861589773</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>8.4821428571428575E-2</v>
+        <v>8.4821428571428577</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>0.58823529411764708</v>
+        <v>58.82352941176471</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1288,15 +1288,15 @@
       </c>
       <c r="M13" s="4">
         <f t="shared" si="0"/>
-        <v>0.22924901185770752</v>
+        <v>22.92490118577075</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
-        <v>0.12887828162291171</v>
+        <v>12.887828162291171</v>
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>0.647887323943662</v>
+        <v>64.788732394366207</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1338,15 +1338,15 @@
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
-        <v>0.27695934001178552</v>
+        <v>27.69593400117855</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>0.37414965986394561</v>
+        <v>37.414965986394563</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0.51428571428571423</v>
+        <v>51.428571428571423</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1388,15 +1388,15 @@
       </c>
       <c r="M15" s="4">
         <f t="shared" si="0"/>
-        <v>0.22073578595317725</v>
+        <v>22.073578595317723</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>0.18215699976706265</v>
+        <v>18.215699976706265</v>
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>0.18181818181818182</v>
+        <v>18.181818181818183</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1438,15 +1438,15 @@
       </c>
       <c r="M16" s="4">
         <f t="shared" si="0"/>
-        <v>0.25964149918522544</v>
+        <v>25.964149918522544</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
-        <v>0.23380992430613962</v>
+        <v>23.380992430613961</v>
       </c>
       <c r="O16">
         <f t="shared" si="2"/>
-        <v>0.2857142857142857</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1488,15 +1488,15 @@
       </c>
       <c r="M17" s="4">
         <f t="shared" si="0"/>
-        <v>0.17716115261472787</v>
+        <v>17.716115261472787</v>
       </c>
       <c r="N17">
         <f t="shared" si="1"/>
-        <v>0.20189818809318377</v>
+        <v>20.189818809318378</v>
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
-        <v>0.54545454545454541</v>
+        <v>54.54545454545454</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1538,15 +1538,15 @@
       </c>
       <c r="M18" s="4">
         <f t="shared" si="0"/>
-        <v>0.17155756207674944</v>
+        <v>17.155756207674944</v>
       </c>
       <c r="N18">
         <f t="shared" si="1"/>
-        <v>0.2471264367816092</v>
+        <v>24.712643678160919</v>
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
-        <v>9.0909090909090912E-2</v>
+        <v>9.0909090909090917</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1588,15 +1588,15 @@
       </c>
       <c r="M19" s="4">
         <f t="shared" si="0"/>
-        <v>0.26281673541543898</v>
+        <v>26.281673541543899</v>
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>0.17651146629603892</v>
+        <v>17.651146629603893</v>
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>0.35897435897435898</v>
+        <v>35.897435897435898</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1638,15 +1638,15 @@
       </c>
       <c r="M20" s="4">
         <f t="shared" si="0"/>
-        <v>0.29596412556053814</v>
+        <v>29.596412556053814</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>9.7460535346602609E-2</v>
+        <v>9.7460535346602608</v>
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>0.29508196721311475</v>
+        <v>29.508196721311474</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1688,15 +1688,15 @@
       </c>
       <c r="M21" s="4">
         <f t="shared" si="0"/>
-        <v>0.2644808743169399</v>
+        <v>26.448087431693988</v>
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>0.17294900221729489</v>
+        <v>17.294900221729488</v>
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>0.53333333333333333</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1738,15 +1738,15 @@
       </c>
       <c r="M22" s="4">
         <f t="shared" si="0"/>
-        <v>0.14987080103359174</v>
+        <v>14.987080103359174</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>6.2308029837648091E-2</v>
+        <v>6.2308029837648089</v>
       </c>
       <c r="O22">
         <f t="shared" si="2"/>
-        <v>-0.26666666666666666</v>
+        <v>-26.666666666666668</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1788,15 +1788,15 @@
       </c>
       <c r="M23" s="4">
         <f t="shared" si="0"/>
-        <v>0.19506272764063132</v>
+        <v>19.50627276406313</v>
       </c>
       <c r="N23">
         <f t="shared" si="1"/>
-        <v>0.16467682173734047</v>
+        <v>16.467682173734048</v>
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
-        <v>-0.47619047619047616</v>
+        <v>-47.619047619047613</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1838,15 +1838,15 @@
       </c>
       <c r="M24" s="4">
         <f t="shared" si="0"/>
-        <v>0.21492537313432836</v>
+        <v>21.492537313432834</v>
       </c>
       <c r="N24">
         <f t="shared" si="1"/>
-        <v>0.1690570643881599</v>
+        <v>16.90570643881599</v>
       </c>
       <c r="O24">
         <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <v>11.111111111111111</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1888,15 +1888,15 @@
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>0.15297982167996246</v>
+        <v>15.297982167996246</v>
       </c>
       <c r="N25">
         <f t="shared" si="1"/>
-        <v>0.20784313725490197</v>
+        <v>20.784313725490197</v>
       </c>
       <c r="O25">
         <f t="shared" si="2"/>
-        <v>6.0606060606060608E-2</v>
+        <v>6.0606060606060606</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1938,15 +1938,15 @@
       </c>
       <c r="M26" s="4">
         <f t="shared" si="0"/>
-        <v>0.26142949130714743</v>
+        <v>26.142949130714744</v>
       </c>
       <c r="N26">
         <f t="shared" si="1"/>
-        <v>6.4876957494407153E-2</v>
+        <v>6.4876957494407153</v>
       </c>
       <c r="O26">
         <f t="shared" si="2"/>
-        <v>0.16</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -1988,15 +1988,15 @@
       </c>
       <c r="M27" s="4">
         <f t="shared" si="0"/>
-        <v>0.23895253682487724</v>
+        <v>23.895253682487724</v>
       </c>
       <c r="N27">
         <f t="shared" si="1"/>
-        <v>0.12989493791786055</v>
+        <v>12.989493791786055</v>
       </c>
       <c r="O27">
         <f t="shared" si="2"/>
-        <v>0.55319148936170215</v>
+        <v>55.319148936170215</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2038,15 +2038,15 @@
       </c>
       <c r="M28" s="4">
         <f t="shared" si="0"/>
-        <v>0.21320973348783315</v>
+        <v>21.320973348783316</v>
       </c>
       <c r="N28">
         <f t="shared" si="1"/>
-        <v>0.25230769230769229</v>
+        <v>25.23076923076923</v>
       </c>
       <c r="O28">
         <f t="shared" si="2"/>
-        <v>0.31111111111111112</v>
+        <v>31.111111111111111</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2088,15 +2088,15 @@
       </c>
       <c r="M29" s="4">
         <f t="shared" si="0"/>
-        <v>0.18416801292407109</v>
+        <v>18.416801292407108</v>
       </c>
       <c r="N29">
         <f t="shared" si="1"/>
-        <v>0.18328840970350405</v>
+        <v>18.328840970350406</v>
       </c>
       <c r="O29">
         <f t="shared" si="2"/>
-        <v>0.46808510638297873</v>
+        <v>46.808510638297875</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2138,15 +2138,15 @@
       </c>
       <c r="M30" s="4">
         <f t="shared" si="0"/>
-        <v>0.22446689113355781</v>
+        <v>22.446689113355781</v>
       </c>
       <c r="N30">
         <f t="shared" si="1"/>
-        <v>0.26473429951690819</v>
+        <v>26.473429951690818</v>
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
-        <v>0.375</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2188,15 +2188,15 @@
       </c>
       <c r="M31" s="4">
         <f t="shared" si="0"/>
-        <v>0.19146919431279621</v>
+        <v>19.14691943127962</v>
       </c>
       <c r="N31">
         <f t="shared" si="1"/>
-        <v>0.21714285714285714</v>
+        <v>21.714285714285715</v>
       </c>
       <c r="O31">
         <f t="shared" si="2"/>
-        <v>0.23255813953488372</v>
+        <v>23.255813953488371</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2238,15 +2238,15 @@
       </c>
       <c r="M32" s="4">
         <f t="shared" si="0"/>
-        <v>0.19584055459272098</v>
+        <v>19.584055459272097</v>
       </c>
       <c r="N32">
         <f t="shared" si="1"/>
-        <v>0.21082441787287604</v>
+        <v>21.082441787287603</v>
       </c>
       <c r="O32">
         <f t="shared" si="2"/>
-        <v>-0.25454545454545452</v>
+        <v>-25.454545454545453</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2288,15 +2288,15 @@
       </c>
       <c r="M33" s="4">
         <f t="shared" si="0"/>
-        <v>0.13286713286713286</v>
+        <v>13.286713286713287</v>
       </c>
       <c r="N33">
         <f t="shared" si="1"/>
-        <v>0.22006472491909385</v>
+        <v>22.006472491909385</v>
       </c>
       <c r="O33">
         <f t="shared" si="2"/>
-        <v>0.31578947368421051</v>
+        <v>31.578947368421051</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2338,15 +2338,15 @@
       </c>
       <c r="M34" s="4">
         <f t="shared" si="0"/>
-        <v>0.16765918460833715</v>
+        <v>16.765918460833714</v>
       </c>
       <c r="N34">
         <f t="shared" si="1"/>
-        <v>0.14068441064638784</v>
+        <v>14.068441064638785</v>
       </c>
       <c r="O34">
         <f t="shared" si="2"/>
-        <v>0.48275862068965519</v>
+        <v>48.275862068965516</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2388,15 +2388,15 @@
       </c>
       <c r="M35" s="4">
         <f t="shared" si="0"/>
-        <v>0.2086677367576244</v>
+        <v>20.866773675762438</v>
       </c>
       <c r="N35">
         <f t="shared" si="1"/>
-        <v>0.17423382519863792</v>
+        <v>17.423382519863793</v>
       </c>
       <c r="O35">
         <f t="shared" si="2"/>
-        <v>9.5238095238095233E-2</v>
+        <v>9.5238095238095237</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2438,15 +2438,15 @@
       </c>
       <c r="M36" s="4">
         <f t="shared" si="0"/>
-        <v>0.22338204592901878</v>
+        <v>22.338204592901878</v>
       </c>
       <c r="N36">
         <f t="shared" si="1"/>
-        <v>0.199288256227758</v>
+        <v>19.9288256227758</v>
       </c>
       <c r="O36">
         <f t="shared" si="2"/>
-        <v>9.5238095238095233E-2</v>
+        <v>9.5238095238095237</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2488,15 +2488,15 @@
       </c>
       <c r="M37" s="4">
         <f t="shared" si="0"/>
-        <v>0.19853709508881923</v>
+        <v>19.853709508881924</v>
       </c>
       <c r="N37">
         <f t="shared" si="1"/>
-        <v>0.22637590861889928</v>
+        <v>22.63759086188993</v>
       </c>
       <c r="O37">
         <f t="shared" si="2"/>
-        <v>0.3783783783783784</v>
+        <v>37.837837837837839</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2538,15 +2538,15 @@
       </c>
       <c r="M38" s="4">
         <f t="shared" si="0"/>
-        <v>0.22300884955752212</v>
+        <v>22.300884955752213</v>
       </c>
       <c r="N38">
         <f t="shared" si="1"/>
-        <v>0.30039525691699603</v>
+        <v>30.039525691699602</v>
       </c>
       <c r="O38">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2588,15 +2588,15 @@
       </c>
       <c r="M39" s="4">
         <f t="shared" si="0"/>
-        <v>0.17987360233349539</v>
+        <v>17.987360233349538</v>
       </c>
       <c r="N39">
         <f t="shared" si="1"/>
-        <v>0.32988165680473375</v>
+        <v>32.988165680473372</v>
       </c>
       <c r="O39">
         <f t="shared" si="2"/>
-        <v>0.47619047619047616</v>
+        <v>47.619047619047613</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2638,15 +2638,15 @@
       </c>
       <c r="M40" s="4">
         <f t="shared" si="0"/>
-        <v>0.22756892230576442</v>
+        <v>22.75689223057644</v>
       </c>
       <c r="N40">
         <f t="shared" si="1"/>
-        <v>0.21001164144353901</v>
+        <v>21.001164144353901</v>
       </c>
       <c r="O40">
         <f t="shared" si="2"/>
-        <v>-5.128205128205128E-2</v>
+        <v>-5.1282051282051277</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2688,15 +2688,15 @@
       </c>
       <c r="M41" s="4">
         <f t="shared" si="0"/>
-        <v>0.15608337372758119</v>
+        <v>15.608337372758118</v>
       </c>
       <c r="N41">
         <f t="shared" si="1"/>
-        <v>0.26133333333333331</v>
+        <v>26.133333333333329</v>
       </c>
       <c r="O41">
         <f t="shared" si="2"/>
-        <v>0.22222222222222221</v>
+        <v>22.222222222222221</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2738,15 +2738,15 @@
       </c>
       <c r="M42" s="4">
         <f t="shared" si="0"/>
-        <v>0.25185185185185183</v>
+        <v>25.185185185185183</v>
       </c>
       <c r="N42">
         <f t="shared" si="1"/>
-        <v>0.12936462507155122</v>
+        <v>12.936462507155122</v>
       </c>
       <c r="O42">
         <f t="shared" si="2"/>
-        <v>4.4444444444444446E-2</v>
+        <v>4.4444444444444446</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2788,15 +2788,15 @@
       </c>
       <c r="M43" s="4">
         <f t="shared" si="0"/>
-        <v>0.16041546451240624</v>
+        <v>16.041546451240624</v>
       </c>
       <c r="N43">
         <f t="shared" si="1"/>
-        <v>0.15873015873015872</v>
+        <v>15.873015873015872</v>
       </c>
       <c r="O43">
         <f t="shared" si="2"/>
-        <v>0.10526315789473684</v>
+        <v>10.526315789473683</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2838,15 +2838,15 @@
       </c>
       <c r="M44" s="4">
         <f t="shared" si="0"/>
-        <v>0.20011841326228538</v>
+        <v>20.011841326228538</v>
       </c>
       <c r="N44">
         <f t="shared" si="1"/>
-        <v>0.18739054290718038</v>
+        <v>18.739054290718038</v>
       </c>
       <c r="O44">
         <f t="shared" si="2"/>
-        <v>0.32558139534883723</v>
+        <v>32.558139534883722</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2888,15 +2888,15 @@
       </c>
       <c r="M45" s="4">
         <f t="shared" si="0"/>
-        <v>0.13928761297182349</v>
+        <v>13.92876129718235</v>
       </c>
       <c r="N45">
         <f t="shared" si="1"/>
-        <v>0.26998583282736288</v>
+        <v>26.998583282736288</v>
       </c>
       <c r="O45">
         <f t="shared" si="2"/>
-        <v>-0.16666666666666666</v>
+        <v>-16.666666666666664</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2938,15 +2938,15 @@
       </c>
       <c r="M46" s="4">
         <f t="shared" si="0"/>
-        <v>0.31646932185145316</v>
+        <v>31.646932185145317</v>
       </c>
       <c r="N46">
         <f t="shared" si="1"/>
-        <v>0.44320297951582865</v>
+        <v>44.320297951582866</v>
       </c>
       <c r="O46">
         <f t="shared" si="2"/>
-        <v>0.2608695652173913</v>
+        <v>26.086956521739129</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -2988,15 +2988,15 @@
       </c>
       <c r="M47" s="4">
         <f t="shared" si="0"/>
-        <v>0.17789203084832905</v>
+        <v>17.789203084832906</v>
       </c>
       <c r="N47">
         <f t="shared" si="1"/>
-        <v>9.2165898617511521E-3</v>
+        <v>0.92165898617511521</v>
       </c>
       <c r="O47">
         <f t="shared" si="2"/>
-        <v>0.94736842105263153</v>
+        <v>94.73684210526315</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -3038,15 +3038,15 @@
       </c>
       <c r="M48" s="4">
         <f t="shared" si="0"/>
-        <v>0.22811671087533156</v>
+        <v>22.811671087533156</v>
       </c>
       <c r="N48">
         <f t="shared" si="1"/>
-        <v>0.17290160326941215</v>
+        <v>17.290160326941216</v>
       </c>
       <c r="O48">
         <f t="shared" si="2"/>
-        <v>-6.8965517241379309E-2</v>
+        <v>-6.8965517241379306</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -3088,15 +3088,15 @@
       </c>
       <c r="M49" s="4">
         <f t="shared" si="0"/>
-        <v>0.21940163191296463</v>
+        <v>21.940163191296463</v>
       </c>
       <c r="N49">
         <f t="shared" si="1"/>
-        <v>0.29925373134328359</v>
+        <v>29.92537313432836</v>
       </c>
       <c r="O49">
         <f t="shared" si="2"/>
-        <v>-2.9850746268656716E-2</v>
+        <v>-2.9850746268656714</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -3138,15 +3138,15 @@
       </c>
       <c r="M50" s="4">
         <f t="shared" si="0"/>
-        <v>0.20413122721749696</v>
+        <v>20.413122721749698</v>
       </c>
       <c r="N50">
         <f t="shared" si="1"/>
-        <v>0.19298245614035087</v>
+        <v>19.298245614035086</v>
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
-        <v>0.13333333333333333</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -3188,15 +3188,15 @@
       </c>
       <c r="M51" s="4">
         <f t="shared" si="0"/>
-        <v>0.14465408805031446</v>
+        <v>14.465408805031446</v>
       </c>
       <c r="N51">
         <f t="shared" si="1"/>
-        <v>0.2617283950617284</v>
+        <v>26.172839506172842</v>
       </c>
       <c r="O51">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>15.384615384615385</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="16.8" x14ac:dyDescent="0.3">
@@ -3238,15 +3238,15 @@
       </c>
       <c r="M52" s="4">
         <f t="shared" si="0"/>
-        <v>0.28293736501079914</v>
+        <v>28.293736501079913</v>
       </c>
       <c r="N52">
         <f t="shared" si="1"/>
-        <v>0.27692307692307694</v>
+        <v>27.692307692307693</v>
       </c>
       <c r="O52">
         <f t="shared" si="2"/>
-        <v>-0.12244897959183673</v>
+        <v>-12.244897959183673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>